<commit_message>
Redid analysis for Ryskin incremental decision run_2 with the new Ryskin data. Finished the Ryskin production pilot experiment. Organized Leffel Et Al files, anonymized MTURK workerids, and added them to the repo
</commit_message>
<xml_diff>
--- a/experiments/RyskinEtAl/2_production/shared/stimuli_creation/list1_production.xlsx
+++ b/experiments/RyskinEtAl/2_production/shared/stimuli_creation/list1_production.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanpophristic/Desktop/Repos/eyetracking_replications/experiments/RyskinEtAl/2_production/shared/stimuli_creation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA58E91B-43D9-354B-A0E0-96469F770626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81045C1-5EE5-B547-BAF9-3C64EEEBADE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27220" yWindow="440" windowWidth="37080" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37080" yWindow="440" windowWidth="37080" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list1_production" sheetId="1" r:id="rId1"/>
@@ -4427,7 +4427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5384,12 +5384,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA290" sqref="AA290"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="114" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L118" sqref="L118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="5" width="10.83203125" style="1"/>
     <col min="6" max="6" width="23.5" style="1" customWidth="1"/>
@@ -5398,9 +5398,17 @@
     <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="14" max="18" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" customWidth="1"/>
+    <col min="20" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="18.1640625" customWidth="1"/>
+    <col min="23" max="23" width="20.33203125" customWidth="1"/>
+    <col min="24" max="26" width="10.83203125" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5480,7 +5488,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5536,7 +5544,7 @@
         <v>13</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>15</v>
@@ -5545,7 +5553,7 @@
         <v>15</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>17</v>
@@ -5560,7 +5568,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -5616,7 +5624,7 @@
         <v>13</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>20</v>
@@ -5628,7 +5636,7 @@
         <v>21</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>1424</v>
@@ -5640,7 +5648,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -5696,7 +5704,7 @@
         <v>13</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>25</v>
@@ -5705,7 +5713,7 @@
         <v>25</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>27</v>
@@ -5720,7 +5728,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5776,7 +5784,7 @@
         <v>13</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>30</v>
@@ -5788,7 +5796,7 @@
         <v>31</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>1424</v>
@@ -5800,7 +5808,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -5856,7 +5864,7 @@
         <v>13</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>35</v>
@@ -5865,7 +5873,7 @@
         <v>35</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="W6" s="3" t="s">
         <v>37</v>
@@ -5880,7 +5888,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -5936,7 +5944,7 @@
         <v>13</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>40</v>
@@ -5948,7 +5956,7 @@
         <v>41</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="X7" s="3" t="s">
         <v>1424</v>
@@ -5960,7 +5968,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -6016,7 +6024,7 @@
         <v>13</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>45</v>
@@ -6025,7 +6033,7 @@
         <v>45</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W8" s="3" t="s">
         <v>47</v>
@@ -6040,7 +6048,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -6096,7 +6104,7 @@
         <v>13</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>50</v>
@@ -6108,7 +6116,7 @@
         <v>51</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="X9" s="3" t="s">
         <v>1424</v>
@@ -6120,7 +6128,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -6176,7 +6184,7 @@
         <v>13</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>55</v>
@@ -6185,7 +6193,7 @@
         <v>55</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W10" s="3" t="s">
         <v>57</v>
@@ -6200,7 +6208,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -6256,7 +6264,7 @@
         <v>13</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>60</v>
@@ -6268,7 +6276,7 @@
         <v>61</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>1424</v>
@@ -6280,7 +6288,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -6297,7 +6305,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>65</v>
@@ -6306,7 +6314,7 @@
         <v>65</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>67</v>
@@ -6360,7 +6368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -6377,7 +6385,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>70</v>
@@ -6389,7 +6397,7 @@
         <v>71</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>1419</v>
@@ -6440,7 +6448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -6457,7 +6465,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>75</v>
@@ -6469,7 +6477,7 @@
         <v>76</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>1419</v>
@@ -6520,7 +6528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -6537,7 +6545,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>80</v>
@@ -6546,7 +6554,7 @@
         <v>80</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>82</v>
@@ -6600,7 +6608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -6617,7 +6625,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>85</v>
@@ -6629,7 +6637,7 @@
         <v>86</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>1419</v>
@@ -6680,7 +6688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -6697,7 +6705,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>90</v>
@@ -6706,7 +6714,7 @@
         <v>90</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>92</v>
@@ -6760,7 +6768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -6777,7 +6785,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>95</v>
@@ -6789,7 +6797,7 @@
         <v>96</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>1419</v>
@@ -6840,7 +6848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -6857,7 +6865,7 @@
         <v>13</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>100</v>
@@ -6866,7 +6874,7 @@
         <v>100</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>102</v>
@@ -6920,7 +6928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -6937,7 +6945,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>105</v>
@@ -6949,7 +6957,7 @@
         <v>106</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>1419</v>
@@ -7000,7 +7008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -7017,7 +7025,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>110</v>
@@ -7026,7 +7034,7 @@
         <v>110</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>112</v>
@@ -7080,7 +7088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -7136,7 +7144,7 @@
         <v>114</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>14</v>
@@ -7148,7 +7156,7 @@
         <v>116</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="X22" s="1" t="s">
         <v>1424</v>
@@ -7160,7 +7168,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -7216,7 +7224,7 @@
         <v>114</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>19</v>
@@ -7225,7 +7233,7 @@
         <v>19</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>121</v>
@@ -7240,7 +7248,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -7296,7 +7304,7 @@
         <v>114</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>24</v>
@@ -7308,7 +7316,7 @@
         <v>124</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>1424</v>
@@ -7320,7 +7328,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -7376,7 +7384,7 @@
         <v>114</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>29</v>
@@ -7385,7 +7393,7 @@
         <v>29</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>129</v>
@@ -7400,7 +7408,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -7456,7 +7464,7 @@
         <v>114</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="T26" s="1" t="s">
         <v>34</v>
@@ -7468,7 +7476,7 @@
         <v>132</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="X26" s="1" t="s">
         <v>1424</v>
@@ -7480,7 +7488,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -7536,7 +7544,7 @@
         <v>114</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="T27" s="1" t="s">
         <v>39</v>
@@ -7545,7 +7553,7 @@
         <v>39</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W27" s="1" t="s">
         <v>137</v>
@@ -7560,7 +7568,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -7616,7 +7624,7 @@
         <v>114</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>44</v>
@@ -7628,7 +7636,7 @@
         <v>140</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X28" s="1" t="s">
         <v>1424</v>
@@ -7640,7 +7648,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -7696,7 +7704,7 @@
         <v>114</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="T29" s="1" t="s">
         <v>49</v>
@@ -7705,7 +7713,7 @@
         <v>49</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="W29" s="1" t="s">
         <v>145</v>
@@ -7720,7 +7728,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -7776,7 +7784,7 @@
         <v>114</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="T30" s="1" t="s">
         <v>54</v>
@@ -7788,7 +7796,7 @@
         <v>148</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="X30" s="1" t="s">
         <v>1424</v>
@@ -7800,7 +7808,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -7856,7 +7864,7 @@
         <v>114</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="T31" s="1" t="s">
         <v>59</v>
@@ -7865,7 +7873,7 @@
         <v>59</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>153</v>
@@ -7880,7 +7888,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -7897,7 +7905,7 @@
         <v>114</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>64</v>
@@ -7909,7 +7917,7 @@
         <v>156</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>1419</v>
@@ -7960,7 +7968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -7977,7 +7985,7 @@
         <v>114</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>69</v>
@@ -7986,7 +7994,7 @@
         <v>69</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>161</v>
@@ -8040,7 +8048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -8057,7 +8065,7 @@
         <v>114</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>74</v>
@@ -8066,7 +8074,7 @@
         <v>74</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>165</v>
@@ -8120,7 +8128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -8137,7 +8145,7 @@
         <v>114</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>79</v>
@@ -8149,7 +8157,7 @@
         <v>168</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>1419</v>
@@ -8200,7 +8208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -8217,7 +8225,7 @@
         <v>114</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>84</v>
@@ -8226,7 +8234,7 @@
         <v>84</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>173</v>
@@ -8280,7 +8288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -8297,7 +8305,7 @@
         <v>114</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>89</v>
@@ -8309,7 +8317,7 @@
         <v>176</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>1419</v>
@@ -8360,7 +8368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -8377,7 +8385,7 @@
         <v>114</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>94</v>
@@ -8386,7 +8394,7 @@
         <v>94</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>181</v>
@@ -8440,7 +8448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -8457,7 +8465,7 @@
         <v>114</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>99</v>
@@ -8469,7 +8477,7 @@
         <v>184</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>1419</v>
@@ -8520,7 +8528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -8537,7 +8545,7 @@
         <v>114</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>104</v>
@@ -8546,7 +8554,7 @@
         <v>104</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>189</v>
@@ -8600,7 +8608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -8617,7 +8625,7 @@
         <v>114</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>109</v>
@@ -8629,7 +8637,7 @@
         <v>192</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>1419</v>
@@ -8680,7 +8688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -8736,7 +8744,7 @@
         <v>13</v>
       </c>
       <c r="S42" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="T42" s="6" t="s">
         <v>197</v>
@@ -8745,7 +8753,7 @@
         <v>198</v>
       </c>
       <c r="V42" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="W42" s="6" t="s">
         <v>200</v>
@@ -8760,7 +8768,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26">
       <c r="A43" s="10">
         <v>42</v>
       </c>
@@ -8816,7 +8824,7 @@
         <v>13</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="T43" s="7" t="s">
         <v>203</v>
@@ -8828,7 +8836,7 @@
         <v>205</v>
       </c>
       <c r="W43" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="X43" s="6" t="s">
         <v>1424</v>
@@ -8840,7 +8848,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -8896,7 +8904,7 @@
         <v>13</v>
       </c>
       <c r="S44" s="7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="T44" s="7" t="s">
         <v>209</v>
@@ -8905,7 +8913,7 @@
         <v>210</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="W44" s="7" t="s">
         <v>212</v>
@@ -8920,7 +8928,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -8976,7 +8984,7 @@
         <v>13</v>
       </c>
       <c r="S45" s="7" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="T45" s="7" t="s">
         <v>215</v>
@@ -8988,7 +8996,7 @@
         <v>217</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="X45" s="6" t="s">
         <v>1424</v>
@@ -9000,7 +9008,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -9056,7 +9064,7 @@
         <v>13</v>
       </c>
       <c r="S46" s="7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="T46" s="7" t="s">
         <v>221</v>
@@ -9065,7 +9073,7 @@
         <v>222</v>
       </c>
       <c r="V46" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="W46" s="7" t="s">
         <v>224</v>
@@ -9080,7 +9088,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26">
       <c r="A47" s="10">
         <v>46</v>
       </c>
@@ -9136,7 +9144,7 @@
         <v>13</v>
       </c>
       <c r="S47" s="7" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="T47" s="7" t="s">
         <v>227</v>
@@ -9148,7 +9156,7 @@
         <v>229</v>
       </c>
       <c r="W47" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="X47" s="6" t="s">
         <v>1424</v>
@@ -9160,7 +9168,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -9216,7 +9224,7 @@
         <v>13</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="T48" s="7" t="s">
         <v>233</v>
@@ -9225,7 +9233,7 @@
         <v>234</v>
       </c>
       <c r="V48" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="W48" s="7" t="s">
         <v>236</v>
@@ -9240,7 +9248,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -9296,7 +9304,7 @@
         <v>13</v>
       </c>
       <c r="S49" s="7" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="T49" s="7" t="s">
         <v>239</v>
@@ -9308,7 +9316,7 @@
         <v>241</v>
       </c>
       <c r="W49" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="X49" s="6" t="s">
         <v>1424</v>
@@ -9320,7 +9328,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26">
       <c r="A50" s="10">
         <v>49</v>
       </c>
@@ -9376,7 +9384,7 @@
         <v>13</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="T50" s="7" t="s">
         <v>245</v>
@@ -9385,7 +9393,7 @@
         <v>246</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="W50" s="7" t="s">
         <v>248</v>
@@ -9400,7 +9408,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26">
       <c r="A51" s="10">
         <v>50</v>
       </c>
@@ -9456,7 +9464,7 @@
         <v>13</v>
       </c>
       <c r="S51" s="7" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="T51" s="7" t="s">
         <v>251</v>
@@ -9468,7 +9476,7 @@
         <v>253</v>
       </c>
       <c r="W51" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="X51" s="6" t="s">
         <v>1424</v>
@@ -9480,7 +9488,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26">
       <c r="A52" s="10">
         <v>51</v>
       </c>
@@ -9536,7 +9544,7 @@
         <v>13</v>
       </c>
       <c r="S52" s="7" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="T52" s="7" t="s">
         <v>257</v>
@@ -9545,7 +9553,7 @@
         <v>258</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="W52" s="7" t="s">
         <v>260</v>
@@ -9560,7 +9568,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26">
       <c r="A53" s="10">
         <v>52</v>
       </c>
@@ -9616,7 +9624,7 @@
         <v>13</v>
       </c>
       <c r="S53" s="7" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="T53" s="7" t="s">
         <v>263</v>
@@ -9628,7 +9636,7 @@
         <v>265</v>
       </c>
       <c r="W53" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="X53" s="6" t="s">
         <v>1424</v>
@@ -9640,7 +9648,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26">
       <c r="A54" s="10">
         <v>53</v>
       </c>
@@ -9696,7 +9704,7 @@
         <v>13</v>
       </c>
       <c r="S54" s="7" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="T54" s="7" t="s">
         <v>269</v>
@@ -9705,7 +9713,7 @@
         <v>270</v>
       </c>
       <c r="V54" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="W54" s="7" t="s">
         <v>272</v>
@@ -9720,7 +9728,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26">
       <c r="A55" s="10">
         <v>54</v>
       </c>
@@ -9776,7 +9784,7 @@
         <v>13</v>
       </c>
       <c r="S55" s="7" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T55" s="7" t="s">
         <v>275</v>
@@ -9788,7 +9796,7 @@
         <v>277</v>
       </c>
       <c r="W55" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="X55" s="6" t="s">
         <v>1424</v>
@@ -9800,7 +9808,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26">
       <c r="A56" s="10">
         <v>55</v>
       </c>
@@ -9856,7 +9864,7 @@
         <v>13</v>
       </c>
       <c r="S56" s="7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="T56" s="7" t="s">
         <v>281</v>
@@ -9865,7 +9873,7 @@
         <v>282</v>
       </c>
       <c r="V56" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="W56" s="7" t="s">
         <v>284</v>
@@ -9880,7 +9888,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26">
       <c r="A57" s="10">
         <v>56</v>
       </c>
@@ -9936,7 +9944,7 @@
         <v>13</v>
       </c>
       <c r="S57" s="7" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="T57" s="7" t="s">
         <v>287</v>
@@ -9948,7 +9956,7 @@
         <v>289</v>
       </c>
       <c r="W57" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="X57" s="6" t="s">
         <v>1424</v>
@@ -9960,7 +9968,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26">
       <c r="A58" s="10">
         <v>57</v>
       </c>
@@ -10016,7 +10024,7 @@
         <v>13</v>
       </c>
       <c r="S58" s="7" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="T58" s="7" t="s">
         <v>293</v>
@@ -10025,7 +10033,7 @@
         <v>294</v>
       </c>
       <c r="V58" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="W58" s="7" t="s">
         <v>296</v>
@@ -10040,7 +10048,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -10096,7 +10104,7 @@
         <v>13</v>
       </c>
       <c r="S59" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="T59" s="7" t="s">
         <v>299</v>
@@ -10108,7 +10116,7 @@
         <v>301</v>
       </c>
       <c r="W59" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="X59" s="6" t="s">
         <v>1424</v>
@@ -10120,7 +10128,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26">
       <c r="A60" s="10">
         <v>59</v>
       </c>
@@ -10176,7 +10184,7 @@
         <v>13</v>
       </c>
       <c r="S60" s="7" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="T60" s="7" t="s">
         <v>305</v>
@@ -10185,7 +10193,7 @@
         <v>306</v>
       </c>
       <c r="V60" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="W60" s="7" t="s">
         <v>308</v>
@@ -10200,7 +10208,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -10256,7 +10264,7 @@
         <v>13</v>
       </c>
       <c r="S61" s="7" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="T61" s="7" t="s">
         <v>311</v>
@@ -10268,7 +10276,7 @@
         <v>313</v>
       </c>
       <c r="W61" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="X61" s="6" t="s">
         <v>1424</v>
@@ -10280,7 +10288,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -10297,7 +10305,7 @@
         <v>13</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>317</v>
@@ -10306,7 +10314,7 @@
         <v>318</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J62" s="7" t="s">
         <v>320</v>
@@ -10360,7 +10368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -10377,7 +10385,7 @@
         <v>13</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>323</v>
@@ -10389,7 +10397,7 @@
         <v>325</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="K63" s="7" t="s">
         <v>1419</v>
@@ -10440,7 +10448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -10457,7 +10465,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>329</v>
@@ -10466,7 +10474,7 @@
         <v>330</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="J64" s="7" t="s">
         <v>332</v>
@@ -10520,7 +10528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -10537,7 +10545,7 @@
         <v>13</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>335</v>
@@ -10549,7 +10557,7 @@
         <v>337</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="K65" s="7" t="s">
         <v>1419</v>
@@ -10600,7 +10608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -10617,7 +10625,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>341</v>
@@ -10626,7 +10634,7 @@
         <v>342</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J66" s="7" t="s">
         <v>344</v>
@@ -10680,7 +10688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -10697,7 +10705,7 @@
         <v>13</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>347</v>
@@ -10709,7 +10717,7 @@
         <v>349</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="K67" s="7" t="s">
         <v>1419</v>
@@ -10760,7 +10768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -10777,7 +10785,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>353</v>
@@ -10786,7 +10794,7 @@
         <v>354</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J68" s="7" t="s">
         <v>356</v>
@@ -10840,7 +10848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -10857,7 +10865,7 @@
         <v>13</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>359</v>
@@ -10869,7 +10877,7 @@
         <v>361</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="K69" s="7" t="s">
         <v>1419</v>
@@ -10920,7 +10928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -10937,7 +10945,7 @@
         <v>13</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>365</v>
@@ -10946,7 +10954,7 @@
         <v>366</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J70" s="7" t="s">
         <v>368</v>
@@ -11000,7 +11008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -11017,7 +11025,7 @@
         <v>13</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>371</v>
@@ -11029,7 +11037,7 @@
         <v>373</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K71" s="7" t="s">
         <v>1419</v>
@@ -11080,7 +11088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -11097,7 +11105,7 @@
         <v>13</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>377</v>
@@ -11106,7 +11114,7 @@
         <v>378</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="J72" s="7" t="s">
         <v>380</v>
@@ -11160,7 +11168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -11177,7 +11185,7 @@
         <v>13</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="G73" s="7" t="s">
         <v>383</v>
@@ -11189,7 +11197,7 @@
         <v>385</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="K73" s="7" t="s">
         <v>1419</v>
@@ -11240,7 +11248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -11257,7 +11265,7 @@
         <v>13</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>389</v>
@@ -11266,7 +11274,7 @@
         <v>390</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J74" s="7" t="s">
         <v>392</v>
@@ -11320,7 +11328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -11337,7 +11345,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>395</v>
@@ -11349,7 +11357,7 @@
         <v>397</v>
       </c>
       <c r="J75" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="K75" s="7" t="s">
         <v>1419</v>
@@ -11400,7 +11408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -11417,7 +11425,7 @@
         <v>13</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="G76" s="7" t="s">
         <v>401</v>
@@ -11426,7 +11434,7 @@
         <v>402</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="J76" s="7" t="s">
         <v>404</v>
@@ -11480,7 +11488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -11497,7 +11505,7 @@
         <v>13</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>407</v>
@@ -11509,7 +11517,7 @@
         <v>409</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="K77" s="7" t="s">
         <v>1419</v>
@@ -11560,7 +11568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -11577,7 +11585,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>413</v>
@@ -11586,7 +11594,7 @@
         <v>414</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="J78" s="7" t="s">
         <v>416</v>
@@ -11640,7 +11648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -11657,7 +11665,7 @@
         <v>13</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>419</v>
@@ -11669,7 +11677,7 @@
         <v>421</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="K79" s="7" t="s">
         <v>1419</v>
@@ -11720,7 +11728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -11737,7 +11745,7 @@
         <v>13</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="G80" s="7" t="s">
         <v>425</v>
@@ -11746,7 +11754,7 @@
         <v>426</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J80" s="7" t="s">
         <v>428</v>
@@ -11800,7 +11808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -11817,7 +11825,7 @@
         <v>13</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>431</v>
@@ -11829,7 +11837,7 @@
         <v>433</v>
       </c>
       <c r="J81" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K81" s="7" t="s">
         <v>1419</v>
@@ -11880,7 +11888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26">
       <c r="A82" s="8">
         <v>81</v>
       </c>
@@ -11936,7 +11944,7 @@
         <v>114</v>
       </c>
       <c r="S82" s="11" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="T82" s="11" t="s">
         <v>196</v>
@@ -11948,7 +11956,7 @@
         <v>438</v>
       </c>
       <c r="W82" s="11" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="X82" s="11" t="s">
         <v>1424</v>
@@ -11960,7 +11968,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26">
       <c r="A83" s="8">
         <v>82</v>
       </c>
@@ -12016,7 +12024,7 @@
         <v>114</v>
       </c>
       <c r="S83" s="11" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="T83" s="11" t="s">
         <v>202</v>
@@ -12025,7 +12033,7 @@
         <v>442</v>
       </c>
       <c r="V83" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="W83" s="11" t="s">
         <v>444</v>
@@ -12040,7 +12048,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26">
       <c r="A84" s="8">
         <v>83</v>
       </c>
@@ -12096,7 +12104,7 @@
         <v>114</v>
       </c>
       <c r="S84" s="11" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="T84" s="11" t="s">
         <v>208</v>
@@ -12108,7 +12116,7 @@
         <v>448</v>
       </c>
       <c r="W84" s="11" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="X84" s="11" t="s">
         <v>1424</v>
@@ -12120,7 +12128,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26">
       <c r="A85" s="8">
         <v>84</v>
       </c>
@@ -12176,7 +12184,7 @@
         <v>114</v>
       </c>
       <c r="S85" s="11" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="T85" s="11" t="s">
         <v>214</v>
@@ -12185,7 +12193,7 @@
         <v>452</v>
       </c>
       <c r="V85" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="W85" s="11" t="s">
         <v>454</v>
@@ -12200,7 +12208,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26">
       <c r="A86" s="8">
         <v>85</v>
       </c>
@@ -12256,7 +12264,7 @@
         <v>114</v>
       </c>
       <c r="S86" s="11" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="T86" s="11" t="s">
         <v>220</v>
@@ -12268,7 +12276,7 @@
         <v>458</v>
       </c>
       <c r="W86" s="11" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="X86" s="11" t="s">
         <v>1424</v>
@@ -12280,7 +12288,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26">
       <c r="A87" s="8">
         <v>86</v>
       </c>
@@ -12336,7 +12344,7 @@
         <v>114</v>
       </c>
       <c r="S87" s="11" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="T87" s="11" t="s">
         <v>226</v>
@@ -12345,7 +12353,7 @@
         <v>462</v>
       </c>
       <c r="V87" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="W87" s="11" t="s">
         <v>464</v>
@@ -12360,7 +12368,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26">
       <c r="A88" s="8">
         <v>87</v>
       </c>
@@ -12416,7 +12424,7 @@
         <v>114</v>
       </c>
       <c r="S88" s="11" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="T88" s="11" t="s">
         <v>232</v>
@@ -12428,7 +12436,7 @@
         <v>468</v>
       </c>
       <c r="W88" s="11" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="X88" s="11" t="s">
         <v>1424</v>
@@ -12440,7 +12448,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26">
       <c r="A89" s="8">
         <v>88</v>
       </c>
@@ -12496,7 +12504,7 @@
         <v>114</v>
       </c>
       <c r="S89" s="11" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="T89" s="11" t="s">
         <v>238</v>
@@ -12505,7 +12513,7 @@
         <v>472</v>
       </c>
       <c r="V89" s="11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="W89" s="11" t="s">
         <v>474</v>
@@ -12520,7 +12528,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26">
       <c r="A90" s="8">
         <v>89</v>
       </c>
@@ -12576,7 +12584,7 @@
         <v>114</v>
       </c>
       <c r="S90" s="11" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="T90" s="11" t="s">
         <v>244</v>
@@ -12588,7 +12596,7 @@
         <v>478</v>
       </c>
       <c r="W90" s="11" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="X90" s="11" t="s">
         <v>1424</v>
@@ -12600,7 +12608,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26">
       <c r="A91" s="8">
         <v>90</v>
       </c>
@@ -12656,7 +12664,7 @@
         <v>114</v>
       </c>
       <c r="S91" s="11" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="T91" s="11" t="s">
         <v>250</v>
@@ -12665,7 +12673,7 @@
         <v>482</v>
       </c>
       <c r="V91" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="W91" s="11" t="s">
         <v>484</v>
@@ -12680,7 +12688,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26">
       <c r="A92" s="8">
         <v>91</v>
       </c>
@@ -12736,7 +12744,7 @@
         <v>114</v>
       </c>
       <c r="S92" s="11" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="T92" s="11" t="s">
         <v>256</v>
@@ -12748,7 +12756,7 @@
         <v>488</v>
       </c>
       <c r="W92" s="11" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="X92" s="11" t="s">
         <v>1424</v>
@@ -12760,7 +12768,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26">
       <c r="A93" s="8">
         <v>92</v>
       </c>
@@ -12816,7 +12824,7 @@
         <v>114</v>
       </c>
       <c r="S93" s="11" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="T93" s="11" t="s">
         <v>262</v>
@@ -12825,7 +12833,7 @@
         <v>492</v>
       </c>
       <c r="V93" s="11" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="W93" s="11" t="s">
         <v>494</v>
@@ -12840,7 +12848,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26">
       <c r="A94" s="8">
         <v>93</v>
       </c>
@@ -12896,7 +12904,7 @@
         <v>114</v>
       </c>
       <c r="S94" s="11" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="T94" s="11" t="s">
         <v>268</v>
@@ -12908,7 +12916,7 @@
         <v>498</v>
       </c>
       <c r="W94" s="11" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="X94" s="11" t="s">
         <v>1424</v>
@@ -12920,7 +12928,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26">
       <c r="A95" s="8">
         <v>94</v>
       </c>
@@ -12976,7 +12984,7 @@
         <v>114</v>
       </c>
       <c r="S95" s="11" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="T95" s="11" t="s">
         <v>274</v>
@@ -12985,7 +12993,7 @@
         <v>502</v>
       </c>
       <c r="V95" s="11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="W95" s="11" t="s">
         <v>504</v>
@@ -13000,7 +13008,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26">
       <c r="A96" s="8">
         <v>95</v>
       </c>
@@ -13056,7 +13064,7 @@
         <v>114</v>
       </c>
       <c r="S96" s="11" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="T96" s="11" t="s">
         <v>280</v>
@@ -13068,7 +13076,7 @@
         <v>508</v>
       </c>
       <c r="W96" s="11" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="X96" s="11" t="s">
         <v>1424</v>
@@ -13080,7 +13088,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26">
       <c r="A97" s="8">
         <v>96</v>
       </c>
@@ -13136,7 +13144,7 @@
         <v>114</v>
       </c>
       <c r="S97" s="11" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="T97" s="11" t="s">
         <v>286</v>
@@ -13145,7 +13153,7 @@
         <v>512</v>
       </c>
       <c r="V97" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="W97" s="11" t="s">
         <v>514</v>
@@ -13160,7 +13168,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26">
       <c r="A98" s="8">
         <v>97</v>
       </c>
@@ -13216,7 +13224,7 @@
         <v>114</v>
       </c>
       <c r="S98" s="11" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="T98" s="11" t="s">
         <v>292</v>
@@ -13228,7 +13236,7 @@
         <v>518</v>
       </c>
       <c r="W98" s="11" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="X98" s="11" t="s">
         <v>1424</v>
@@ -13240,7 +13248,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:26">
       <c r="A99" s="8">
         <v>98</v>
       </c>
@@ -13296,7 +13304,7 @@
         <v>114</v>
       </c>
       <c r="S99" s="11" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="T99" s="11" t="s">
         <v>298</v>
@@ -13305,7 +13313,7 @@
         <v>522</v>
       </c>
       <c r="V99" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="W99" s="11" t="s">
         <v>524</v>
@@ -13320,7 +13328,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:26">
       <c r="A100" s="8">
         <v>99</v>
       </c>
@@ -13376,7 +13384,7 @@
         <v>114</v>
       </c>
       <c r="S100" s="11" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="T100" s="11" t="s">
         <v>304</v>
@@ -13388,7 +13396,7 @@
         <v>528</v>
       </c>
       <c r="W100" s="11" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="X100" s="11" t="s">
         <v>1424</v>
@@ -13400,7 +13408,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:26">
       <c r="A101" s="8">
         <v>100</v>
       </c>
@@ -13456,7 +13464,7 @@
         <v>114</v>
       </c>
       <c r="S101" s="11" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="T101" s="11" t="s">
         <v>310</v>
@@ -13465,7 +13473,7 @@
         <v>532</v>
       </c>
       <c r="V101" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="W101" s="11" t="s">
         <v>534</v>
@@ -13480,7 +13488,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:26">
       <c r="A102" s="11">
         <v>101</v>
       </c>
@@ -13497,7 +13505,7 @@
         <v>114</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>316</v>
@@ -13509,7 +13517,7 @@
         <v>538</v>
       </c>
       <c r="J102" s="11" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="K102" s="11" t="s">
         <v>1419</v>
@@ -13560,7 +13568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:26">
       <c r="A103" s="11">
         <v>102</v>
       </c>
@@ -13577,7 +13585,7 @@
         <v>114</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>322</v>
@@ -13586,7 +13594,7 @@
         <v>542</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J103" s="11" t="s">
         <v>544</v>
@@ -13640,7 +13648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26">
       <c r="A104" s="11">
         <v>103</v>
       </c>
@@ -13657,7 +13665,7 @@
         <v>114</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>328</v>
@@ -13669,7 +13677,7 @@
         <v>548</v>
       </c>
       <c r="J104" s="11" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="K104" s="11" t="s">
         <v>1419</v>
@@ -13720,7 +13728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26">
       <c r="A105" s="11">
         <v>104</v>
       </c>
@@ -13737,7 +13745,7 @@
         <v>114</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>334</v>
@@ -13746,7 +13754,7 @@
         <v>552</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J105" s="11" t="s">
         <v>554</v>
@@ -13800,7 +13808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:26">
       <c r="A106" s="11">
         <v>105</v>
       </c>
@@ -13817,7 +13825,7 @@
         <v>114</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>340</v>
@@ -13829,7 +13837,7 @@
         <v>558</v>
       </c>
       <c r="J106" s="11" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="K106" s="11" t="s">
         <v>1419</v>
@@ -13880,7 +13888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:26">
       <c r="A107" s="11">
         <v>106</v>
       </c>
@@ -13897,7 +13905,7 @@
         <v>114</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>346</v>
@@ -13906,7 +13914,7 @@
         <v>562</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J107" s="11" t="s">
         <v>564</v>
@@ -13960,7 +13968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26">
       <c r="A108" s="11">
         <v>107</v>
       </c>
@@ -13977,7 +13985,7 @@
         <v>114</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>352</v>
@@ -13989,7 +13997,7 @@
         <v>568</v>
       </c>
       <c r="J108" s="11" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="K108" s="11" t="s">
         <v>1419</v>
@@ -14040,7 +14048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:26">
       <c r="A109" s="11">
         <v>108</v>
       </c>
@@ -14057,7 +14065,7 @@
         <v>114</v>
       </c>
       <c r="F109" s="11" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="G109" s="11" t="s">
         <v>358</v>
@@ -14066,7 +14074,7 @@
         <v>572</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="J109" s="11" t="s">
         <v>574</v>
@@ -14120,7 +14128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:26">
       <c r="A110" s="11">
         <v>109</v>
       </c>
@@ -14137,7 +14145,7 @@
         <v>114</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>364</v>
@@ -14149,7 +14157,7 @@
         <v>578</v>
       </c>
       <c r="J110" s="11" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="K110" s="11" t="s">
         <v>1419</v>
@@ -14200,7 +14208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:26">
       <c r="A111" s="11">
         <v>110</v>
       </c>
@@ -14217,7 +14225,7 @@
         <v>114</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>370</v>
@@ -14226,7 +14234,7 @@
         <v>582</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J111" s="11" t="s">
         <v>584</v>
@@ -14280,7 +14288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:26">
       <c r="A112" s="11">
         <v>111</v>
       </c>
@@ -14297,7 +14305,7 @@
         <v>114</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>376</v>
@@ -14309,7 +14317,7 @@
         <v>588</v>
       </c>
       <c r="J112" s="11" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="K112" s="11" t="s">
         <v>1419</v>
@@ -14360,7 +14368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:26">
       <c r="A113" s="11">
         <v>112</v>
       </c>
@@ -14377,7 +14385,7 @@
         <v>114</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>382</v>
@@ -14386,7 +14394,7 @@
         <v>592</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="J113" s="11" t="s">
         <v>594</v>
@@ -14440,7 +14448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:26">
       <c r="A114" s="11">
         <v>113</v>
       </c>
@@ -14457,7 +14465,7 @@
         <v>114</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>388</v>
@@ -14469,7 +14477,7 @@
         <v>598</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="K114" s="11" t="s">
         <v>1419</v>
@@ -14520,7 +14528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:26">
       <c r="A115" s="11">
         <v>114</v>
       </c>
@@ -14537,7 +14545,7 @@
         <v>114</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="G115" s="11" t="s">
         <v>394</v>
@@ -14546,7 +14554,7 @@
         <v>602</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="J115" s="11" t="s">
         <v>604</v>
@@ -14600,7 +14608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:26">
       <c r="A116" s="11">
         <v>115</v>
       </c>
@@ -14617,7 +14625,7 @@
         <v>114</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>400</v>
@@ -14629,7 +14637,7 @@
         <v>608</v>
       </c>
       <c r="J116" s="11" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="K116" s="11" t="s">
         <v>1419</v>
@@ -14680,7 +14688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:26">
       <c r="A117" s="11">
         <v>116</v>
       </c>
@@ -14697,7 +14705,7 @@
         <v>114</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="G117" s="11" t="s">
         <v>406</v>
@@ -14706,7 +14714,7 @@
         <v>612</v>
       </c>
       <c r="I117" s="11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J117" s="11" t="s">
         <v>614</v>
@@ -14760,7 +14768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:26">
       <c r="A118" s="11">
         <v>117</v>
       </c>
@@ -14777,7 +14785,7 @@
         <v>114</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="G118" s="11" t="s">
         <v>412</v>
@@ -14789,7 +14797,7 @@
         <v>618</v>
       </c>
       <c r="J118" s="11" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="K118" s="11" t="s">
         <v>1419</v>
@@ -14840,7 +14848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:26">
       <c r="A119" s="11">
         <v>118</v>
       </c>
@@ -14857,7 +14865,7 @@
         <v>114</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="G119" s="11" t="s">
         <v>418</v>
@@ -14866,7 +14874,7 @@
         <v>622</v>
       </c>
       <c r="I119" s="11" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="J119" s="11" t="s">
         <v>624</v>
@@ -14920,7 +14928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:26">
       <c r="A120" s="11">
         <v>119</v>
       </c>
@@ -14937,7 +14945,7 @@
         <v>114</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="G120" s="11" t="s">
         <v>424</v>
@@ -14949,7 +14957,7 @@
         <v>628</v>
       </c>
       <c r="J120" s="11" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="K120" s="11" t="s">
         <v>1419</v>
@@ -15000,7 +15008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:26">
       <c r="A121" s="11">
         <v>120</v>
       </c>
@@ -15017,7 +15025,7 @@
         <v>114</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>430</v>
@@ -15026,7 +15034,7 @@
         <v>632</v>
       </c>
       <c r="I121" s="11" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="J121" s="11" t="s">
         <v>634</v>
@@ -15080,7 +15088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:26">
       <c r="A122" s="12">
         <v>121</v>
       </c>
@@ -15160,7 +15168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:26">
       <c r="A123" s="12">
         <v>122</v>
       </c>
@@ -15240,7 +15248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:26">
       <c r="A124" s="12">
         <v>123</v>
       </c>
@@ -15320,7 +15328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:26">
       <c r="A125" s="12">
         <v>124</v>
       </c>
@@ -15400,7 +15408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:26">
       <c r="A126" s="12">
         <v>125</v>
       </c>
@@ -15480,7 +15488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:26">
       <c r="A127" s="12">
         <v>126</v>
       </c>
@@ -15560,7 +15568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:26">
       <c r="A128" s="12">
         <v>127</v>
       </c>
@@ -15640,7 +15648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:26">
       <c r="A129" s="12">
         <v>128</v>
       </c>
@@ -15720,7 +15728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:26">
       <c r="A130" s="12">
         <v>129</v>
       </c>
@@ -15800,7 +15808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:26">
       <c r="A131" s="12">
         <v>130</v>
       </c>
@@ -15880,7 +15888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:26">
       <c r="A132" s="12">
         <v>131</v>
       </c>
@@ -15960,7 +15968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:26">
       <c r="A133" s="12">
         <v>132</v>
       </c>
@@ -16040,7 +16048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:26">
       <c r="A134" s="12">
         <v>133</v>
       </c>
@@ -16120,7 +16128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:26">
       <c r="A135" s="12">
         <v>134</v>
       </c>
@@ -16200,7 +16208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:26">
       <c r="A136" s="12">
         <v>135</v>
       </c>
@@ -16280,7 +16288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:26">
       <c r="A137" s="12">
         <v>136</v>
       </c>
@@ -16360,7 +16368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:26">
       <c r="A138" s="12">
         <v>137</v>
       </c>
@@ -16440,7 +16448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:26">
       <c r="A139" s="12">
         <v>138</v>
       </c>
@@ -16520,7 +16528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:26">
       <c r="A140" s="12">
         <v>139</v>
       </c>
@@ -16600,7 +16608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:26">
       <c r="A141" s="12">
         <v>140</v>
       </c>
@@ -16680,7 +16688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:26">
       <c r="A142" s="12">
         <v>141</v>
       </c>
@@ -16760,7 +16768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:26">
       <c r="A143" s="12">
         <v>142</v>
       </c>
@@ -16840,7 +16848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:26">
       <c r="A144" s="12">
         <v>143</v>
       </c>
@@ -16920,7 +16928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:26">
       <c r="A145" s="12">
         <v>144</v>
       </c>
@@ -17000,7 +17008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:26">
       <c r="A146" s="12">
         <v>145</v>
       </c>
@@ -17080,7 +17088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:26">
       <c r="A147" s="12">
         <v>146</v>
       </c>
@@ -17160,7 +17168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:26">
       <c r="A148" s="12">
         <v>147</v>
       </c>
@@ -17240,7 +17248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:26">
       <c r="A149" s="12">
         <v>148</v>
       </c>
@@ -17320,7 +17328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:26">
       <c r="A150" s="12">
         <v>149</v>
       </c>
@@ -17400,7 +17408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:26">
       <c r="A151" s="12">
         <v>150</v>
       </c>
@@ -17480,7 +17488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:26">
       <c r="A152" s="12">
         <v>151</v>
       </c>
@@ -17560,7 +17568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:26">
       <c r="A153" s="12">
         <v>152</v>
       </c>
@@ -17640,7 +17648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:26">
       <c r="A154" s="12">
         <v>153</v>
       </c>
@@ -17720,7 +17728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:26">
       <c r="A155" s="12">
         <v>154</v>
       </c>
@@ -17800,7 +17808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:26">
       <c r="A156" s="12">
         <v>155</v>
       </c>
@@ -17880,7 +17888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:26">
       <c r="A157" s="12">
         <v>156</v>
       </c>
@@ -17960,7 +17968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:26">
       <c r="A158" s="12">
         <v>157</v>
       </c>
@@ -18040,7 +18048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:26">
       <c r="A159" s="12">
         <v>158</v>
       </c>
@@ -18120,7 +18128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:26">
       <c r="A160" s="12">
         <v>159</v>
       </c>
@@ -18200,7 +18208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:26">
       <c r="A161" s="12">
         <v>160</v>
       </c>
@@ -18280,7 +18288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:26">
       <c r="A162" s="12">
         <v>161</v>
       </c>
@@ -18360,7 +18368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:26">
       <c r="A163" s="12">
         <v>162</v>
       </c>
@@ -18440,7 +18448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:26">
       <c r="A164" s="12">
         <v>163</v>
       </c>
@@ -18520,7 +18528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:26">
       <c r="A165" s="12">
         <v>164</v>
       </c>
@@ -18600,7 +18608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:26">
       <c r="A166" s="12">
         <v>165</v>
       </c>
@@ -18680,7 +18688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:26">
       <c r="A167" s="12">
         <v>166</v>
       </c>
@@ -18760,7 +18768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:26">
       <c r="A168" s="12">
         <v>167</v>
       </c>
@@ -18840,7 +18848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:26">
       <c r="A169" s="12">
         <v>168</v>
       </c>
@@ -18920,7 +18928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:26">
       <c r="A170" s="12">
         <v>169</v>
       </c>
@@ -19000,7 +19008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:26">
       <c r="A171" s="12">
         <v>170</v>
       </c>
@@ -19080,7 +19088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:26">
       <c r="A172" s="12">
         <v>171</v>
       </c>
@@ -19160,7 +19168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:26">
       <c r="A173" s="12">
         <v>172</v>
       </c>
@@ -19240,7 +19248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:26">
       <c r="A174" s="12">
         <v>173</v>
       </c>
@@ -19320,7 +19328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:26">
       <c r="A175" s="12">
         <v>174</v>
       </c>
@@ -19400,7 +19408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:26">
       <c r="A176" s="12">
         <v>175</v>
       </c>
@@ -19480,7 +19488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:26">
       <c r="A177" s="12">
         <v>176</v>
       </c>
@@ -19560,7 +19568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:26">
       <c r="A178" s="12">
         <v>177</v>
       </c>
@@ -19640,7 +19648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:26">
       <c r="A179" s="12">
         <v>178</v>
       </c>
@@ -19720,7 +19728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:26">
       <c r="A180" s="12">
         <v>179</v>
       </c>
@@ -19800,7 +19808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:26">
       <c r="A181" s="12">
         <v>180</v>
       </c>
@@ -19880,7 +19888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:26">
       <c r="A182" s="12">
         <v>181</v>
       </c>
@@ -19960,7 +19968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:26">
       <c r="A183" s="12">
         <v>182</v>
       </c>
@@ -20040,7 +20048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:26">
       <c r="A184" s="12">
         <v>183</v>
       </c>
@@ -20120,7 +20128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:26">
       <c r="A185" s="12">
         <v>184</v>
       </c>
@@ -20200,7 +20208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:26">
       <c r="A186" s="12">
         <v>185</v>
       </c>
@@ -20280,7 +20288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:26">
       <c r="A187" s="12">
         <v>186</v>
       </c>
@@ -20360,7 +20368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:26">
       <c r="A188" s="12">
         <v>187</v>
       </c>
@@ -20440,7 +20448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:26">
       <c r="A189" s="12">
         <v>188</v>
       </c>
@@ -20520,7 +20528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:26">
       <c r="A190" s="12">
         <v>189</v>
       </c>
@@ -20600,7 +20608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:26">
       <c r="A191" s="12">
         <v>190</v>
       </c>
@@ -20680,7 +20688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:26">
       <c r="A192" s="12">
         <v>191</v>
       </c>
@@ -20760,7 +20768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:26">
       <c r="A193" s="12">
         <v>192</v>
       </c>
@@ -20840,7 +20848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:26">
       <c r="A194" s="12">
         <v>193</v>
       </c>
@@ -20920,7 +20928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:26">
       <c r="A195" s="12">
         <v>194</v>
       </c>
@@ -21000,7 +21008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:26">
       <c r="A196" s="12">
         <v>195</v>
       </c>
@@ -21080,7 +21088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:26">
       <c r="A197" s="12">
         <v>196</v>
       </c>
@@ -21160,7 +21168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:26">
       <c r="A198" s="12">
         <v>197</v>
       </c>
@@ -21240,7 +21248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:26">
       <c r="A199" s="12">
         <v>198</v>
       </c>
@@ -21320,7 +21328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:26">
       <c r="A200" s="12">
         <v>199</v>
       </c>
@@ -21400,7 +21408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:26">
       <c r="A201" s="12">
         <v>200</v>
       </c>
@@ -21480,7 +21488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:26">
       <c r="A202" s="12">
         <v>201</v>
       </c>
@@ -21560,7 +21568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="203" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:26">
       <c r="A203" s="12">
         <v>202</v>
       </c>
@@ -21640,7 +21648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="204" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:26">
       <c r="A204" s="12">
         <v>203</v>
       </c>
@@ -21720,7 +21728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="205" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:26">
       <c r="A205" s="12">
         <v>204</v>
       </c>
@@ -21800,7 +21808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="206" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:26">
       <c r="A206" s="12">
         <v>205</v>
       </c>
@@ -21880,7 +21888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="207" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:26">
       <c r="A207" s="12">
         <v>206</v>
       </c>
@@ -21960,7 +21968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="208" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:26">
       <c r="A208" s="12">
         <v>207</v>
       </c>
@@ -22040,7 +22048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="209" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:26">
       <c r="A209" s="12">
         <v>208</v>
       </c>
@@ -22120,7 +22128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="210" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:26">
       <c r="A210" s="12">
         <v>209</v>
       </c>
@@ -22200,7 +22208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="211" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:26">
       <c r="A211" s="12">
         <v>210</v>
       </c>
@@ -22280,7 +22288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="212" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:26">
       <c r="A212" s="12">
         <v>211</v>
       </c>
@@ -22360,7 +22368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="213" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:26">
       <c r="A213" s="12">
         <v>212</v>
       </c>
@@ -22440,7 +22448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="214" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:26">
       <c r="A214" s="12">
         <v>213</v>
       </c>
@@ -22520,7 +22528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="215" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:26">
       <c r="A215" s="12">
         <v>214</v>
       </c>
@@ -22600,7 +22608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="216" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:26">
       <c r="A216" s="12">
         <v>215</v>
       </c>
@@ -22680,7 +22688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="217" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:26">
       <c r="A217" s="12">
         <v>216</v>
       </c>
@@ -22760,7 +22768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="218" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:26">
       <c r="A218" s="12">
         <v>217</v>
       </c>
@@ -22840,7 +22848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="219" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:26">
       <c r="A219" s="12">
         <v>218</v>
       </c>
@@ -22920,7 +22928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="220" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:26">
       <c r="A220" s="12">
         <v>219</v>
       </c>
@@ -23000,7 +23008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="221" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:26">
       <c r="A221" s="12">
         <v>220</v>
       </c>
@@ -23080,7 +23088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="222" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:26">
       <c r="A222" s="12">
         <v>221</v>
       </c>
@@ -23160,7 +23168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="223" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:26">
       <c r="A223" s="12">
         <v>222</v>
       </c>
@@ -23240,7 +23248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="224" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:26">
       <c r="A224" s="12">
         <v>223</v>
       </c>
@@ -23320,7 +23328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="225" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:26">
       <c r="A225" s="12">
         <v>224</v>
       </c>
@@ -23400,7 +23408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="226" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:26">
       <c r="A226" s="12">
         <v>225</v>
       </c>
@@ -23480,7 +23488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="227" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:26">
       <c r="A227" s="12">
         <v>226</v>
       </c>
@@ -23560,7 +23568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="228" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:26">
       <c r="A228" s="12">
         <v>227</v>
       </c>
@@ -23640,7 +23648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="229" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:26">
       <c r="A229" s="12">
         <v>228</v>
       </c>
@@ -23720,7 +23728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="230" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:26">
       <c r="A230" s="12">
         <v>229</v>
       </c>
@@ -23800,7 +23808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="231" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:26">
       <c r="A231" s="12">
         <v>230</v>
       </c>
@@ -23880,7 +23888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="232" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:26">
       <c r="A232" s="12">
         <v>231</v>
       </c>
@@ -23960,7 +23968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="233" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:26">
       <c r="A233" s="12">
         <v>232</v>
       </c>
@@ -24040,7 +24048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="234" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:26">
       <c r="A234" s="12">
         <v>233</v>
       </c>
@@ -24120,7 +24128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="235" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:26">
       <c r="A235" s="12">
         <v>234</v>
       </c>
@@ -24200,7 +24208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="236" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:26">
       <c r="A236" s="12">
         <v>235</v>
       </c>
@@ -24280,7 +24288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="237" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:26">
       <c r="A237" s="12">
         <v>236</v>
       </c>
@@ -24360,7 +24368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="238" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:26">
       <c r="A238" s="12">
         <v>237</v>
       </c>
@@ -24440,7 +24448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="239" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:26">
       <c r="A239" s="12">
         <v>238</v>
       </c>
@@ -24520,7 +24528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="240" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:26">
       <c r="A240" s="12">
         <v>239</v>
       </c>
@@ -24600,7 +24608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="241" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:26">
       <c r="A241" s="12">
         <v>240</v>
       </c>
@@ -24680,7 +24688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="242" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:26">
       <c r="A242" s="12">
         <v>241</v>
       </c>
@@ -24760,7 +24768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="243" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:26">
       <c r="A243" s="12">
         <v>242</v>
       </c>
@@ -24840,7 +24848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="244" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:26">
       <c r="A244" s="12">
         <v>243</v>
       </c>
@@ -24920,7 +24928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="245" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:26">
       <c r="A245" s="12">
         <v>244</v>
       </c>
@@ -25000,7 +25008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="246" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:26">
       <c r="A246" s="12">
         <v>245</v>
       </c>
@@ -25080,7 +25088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="247" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:26">
       <c r="A247" s="12">
         <v>246</v>
       </c>
@@ -25160,7 +25168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="248" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:26">
       <c r="A248" s="12">
         <v>247</v>
       </c>
@@ -25240,7 +25248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="249" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:26">
       <c r="A249" s="12">
         <v>248</v>
       </c>
@@ -25320,7 +25328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="250" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:26">
       <c r="A250" s="12">
         <v>249</v>
       </c>
@@ -25400,7 +25408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="251" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:26">
       <c r="A251" s="12">
         <v>250</v>
       </c>
@@ -25480,7 +25488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:26">
       <c r="A252" s="12">
         <v>251</v>
       </c>
@@ -25560,7 +25568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="253" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:26">
       <c r="A253" s="12">
         <v>252</v>
       </c>
@@ -25640,7 +25648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="254" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:26">
       <c r="A254" s="12">
         <v>253</v>
       </c>
@@ -25720,7 +25728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="255" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:26">
       <c r="A255" s="12">
         <v>254</v>
       </c>
@@ -25800,7 +25808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="256" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:26">
       <c r="A256" s="12">
         <v>255</v>
       </c>
@@ -25880,7 +25888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="257" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:26">
       <c r="A257" s="12">
         <v>256</v>
       </c>
@@ -25960,7 +25968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="258" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:26">
       <c r="A258" s="12">
         <v>257</v>
       </c>
@@ -26040,7 +26048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="259" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:26">
       <c r="A259" s="12">
         <v>258</v>
       </c>
@@ -26120,7 +26128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="260" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:26">
       <c r="A260" s="12">
         <v>259</v>
       </c>
@@ -26200,7 +26208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="261" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:26">
       <c r="A261" s="12">
         <v>260</v>
       </c>
@@ -26280,7 +26288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="262" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:26">
       <c r="A262" s="12">
         <v>261</v>
       </c>
@@ -26360,7 +26368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="263" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:26">
       <c r="A263" s="12">
         <v>262</v>
       </c>
@@ -26440,7 +26448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="264" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:26">
       <c r="A264" s="12">
         <v>263</v>
       </c>
@@ -26520,7 +26528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="265" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:26">
       <c r="A265" s="12">
         <v>264</v>
       </c>
@@ -26600,7 +26608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="266" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:26">
       <c r="A266" s="12">
         <v>265</v>
       </c>
@@ -26680,7 +26688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="267" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:26">
       <c r="A267" s="12">
         <v>266</v>
       </c>
@@ -26760,7 +26768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="268" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:26">
       <c r="A268" s="12">
         <v>267</v>
       </c>
@@ -26840,7 +26848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="269" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:26">
       <c r="A269" s="12">
         <v>268</v>
       </c>
@@ -26920,7 +26928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="270" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:26">
       <c r="A270" s="12">
         <v>269</v>
       </c>
@@ -27000,7 +27008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="271" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:26">
       <c r="A271" s="12">
         <v>270</v>
       </c>
@@ -27080,7 +27088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="272" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:26">
       <c r="A272" s="12">
         <v>271</v>
       </c>
@@ -27160,7 +27168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="273" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:26">
       <c r="A273" s="12">
         <v>272</v>
       </c>
@@ -27240,7 +27248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="274" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:26">
       <c r="A274" s="12">
         <v>273</v>
       </c>
@@ -27320,7 +27328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="275" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:26">
       <c r="A275" s="12">
         <v>274</v>
       </c>
@@ -27400,7 +27408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="276" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:26">
       <c r="A276" s="12">
         <v>275</v>
       </c>
@@ -27480,7 +27488,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="277" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:26">
       <c r="A277" s="12">
         <v>276</v>
       </c>
@@ -27560,7 +27568,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="278" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:26">
       <c r="A278" s="12">
         <v>277</v>
       </c>
@@ -27640,7 +27648,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="279" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:26">
       <c r="A279" s="12">
         <v>278</v>
       </c>
@@ -27720,7 +27728,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="280" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:26">
       <c r="A280" s="12">
         <v>279</v>
       </c>
@@ -27800,7 +27808,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="281" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:26">
       <c r="A281" s="12">
         <v>280</v>
       </c>
@@ -27880,7 +27888,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="282" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:26">
       <c r="A282" s="12">
         <v>281</v>
       </c>
@@ -27960,7 +27968,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="283" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:26">
       <c r="A283" s="12">
         <v>282</v>
       </c>
@@ -28040,7 +28048,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="284" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:26">
       <c r="A284" s="12">
         <v>283</v>
       </c>
@@ -28120,7 +28128,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="285" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:26">
       <c r="A285" s="12">
         <v>284</v>
       </c>
@@ -28200,7 +28208,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="286" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:26">
       <c r="A286" s="12">
         <v>285</v>
       </c>
@@ -28280,7 +28288,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="287" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:26">
       <c r="A287" s="12">
         <v>286</v>
       </c>
@@ -28360,7 +28368,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="288" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:26">
       <c r="A288" s="12">
         <v>287</v>
       </c>
@@ -28440,7 +28448,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="289" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:26">
       <c r="A289" s="12">
         <v>288</v>
       </c>
@@ -28520,7 +28528,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="290" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:26">
       <c r="A290" s="12">
         <v>289</v>
       </c>
@@ -28600,7 +28608,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="291" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:26">
       <c r="A291" s="12">
         <v>290</v>
       </c>
@@ -28680,7 +28688,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="292" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:26">
       <c r="A292" s="12">
         <v>291</v>
       </c>
@@ -28760,7 +28768,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="293" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:26">
       <c r="A293" s="12">
         <v>292</v>
       </c>
@@ -28840,7 +28848,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="294" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:26">
       <c r="A294" s="12">
         <v>293</v>
       </c>
@@ -28920,7 +28928,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="295" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:26">
       <c r="A295" s="12">
         <v>294</v>
       </c>
@@ -29000,7 +29008,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="296" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:26">
       <c r="A296" s="12">
         <v>295</v>
       </c>
@@ -29080,7 +29088,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="297" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:26">
       <c r="A297" s="12">
         <v>296</v>
       </c>
@@ -29160,7 +29168,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="298" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:26">
       <c r="A298" s="12">
         <v>297</v>
       </c>
@@ -29240,7 +29248,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="299" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:26">
       <c r="A299" s="12">
         <v>298</v>
       </c>
@@ -29320,7 +29328,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="300" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:26">
       <c r="A300" s="12">
         <v>299</v>
       </c>
@@ -29400,7 +29408,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="301" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:26">
       <c r="A301" s="12">
         <v>300</v>
       </c>

</xml_diff>